<commit_message>
Sıralama ve Filtreleme konusu eklendi
</commit_message>
<xml_diff>
--- a/Veri_Setleri/imdb.xlsx
+++ b/Veri_Setleri/imdb.xlsx
@@ -88,10 +88,10 @@
     <t xml:space="preserve">Seven Samurai </t>
   </si>
   <si>
-    <t xml:space="preserve">Inception </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Star Wars </t>
+    <t xml:space="preserve">Inception</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Star Wars</t>
   </si>
   <si>
     <t xml:space="preserve">Forrest Gump </t>
@@ -812,11 +812,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -837,6 +838,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -881,7 +889,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -890,8 +898,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -913,30 +929,30 @@
   </sheetPr>
   <dimension ref="A1:D248"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="59.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -947,10 +963,10 @@
       <c r="B2" s="0" t="n">
         <v>1994</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="4" t="n">
         <v>1071904</v>
       </c>
     </row>
@@ -961,10 +977,10 @@
       <c r="B3" s="0" t="n">
         <v>1972</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="4" t="n">
         <v>751381</v>
       </c>
     </row>
@@ -978,7 +994,7 @@
       <c r="C4" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="4" t="n">
         <v>488889</v>
       </c>
     </row>
@@ -989,10 +1005,10 @@
       <c r="B5" s="0" t="n">
         <v>1994</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="4" t="n">
         <v>830504</v>
       </c>
     </row>
@@ -1003,10 +1019,10 @@
       <c r="B6" s="0" t="n">
         <v>2008</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="4" t="n">
         <v>1045186</v>
       </c>
     </row>
@@ -1017,10 +1033,10 @@
       <c r="B7" s="0" t="n">
         <v>1957</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="4" t="n">
         <v>264112</v>
       </c>
     </row>
@@ -1031,10 +1047,10 @@
       <c r="B8" s="0" t="n">
         <v>1993</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="4" t="n">
         <v>545703</v>
       </c>
     </row>
@@ -1045,10 +1061,10 @@
       <c r="B9" s="0" t="n">
         <v>2003</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="4" t="n">
         <v>758388</v>
       </c>
     </row>
@@ -1059,10 +1075,10 @@
       <c r="B10" s="0" t="n">
         <v>1999</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="4" t="n">
         <v>814389</v>
       </c>
     </row>
@@ -1073,10 +1089,10 @@
       <c r="B11" s="0" t="n">
         <v>1980</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="4" t="n">
         <v>519895</v>
       </c>
     </row>
@@ -1087,10 +1103,10 @@
       <c r="B12" s="0" t="n">
         <v>2001</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="4" t="n">
         <v>784999</v>
       </c>
     </row>
@@ -1101,10 +1117,10 @@
       <c r="B13" s="0" t="n">
         <v>1975</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="4" t="n">
         <v>447005</v>
       </c>
     </row>
@@ -1115,10 +1131,10 @@
       <c r="B14" s="0" t="n">
         <v>1990</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="4" t="n">
         <v>465445</v>
       </c>
     </row>
@@ -1129,10 +1145,10 @@
       <c r="B15" s="0" t="n">
         <v>1954</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="4" t="n">
         <v>161969</v>
       </c>
     </row>
@@ -1143,10 +1159,10 @@
       <c r="B16" s="0" t="n">
         <v>2010</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="4" t="n">
         <v>844938</v>
       </c>
     </row>
@@ -1157,10 +1173,10 @@
       <c r="B17" s="0" t="n">
         <v>1977</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="4" t="n">
         <v>585132</v>
       </c>
     </row>
@@ -1171,10 +1187,10 @@
       <c r="B18" s="0" t="n">
         <v>1994</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="4" t="n">
         <v>711386</v>
       </c>
     </row>
@@ -1185,10 +1201,10 @@
       <c r="B19" s="0" t="n">
         <v>1999</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="4" t="n">
         <v>770559</v>
       </c>
     </row>
@@ -1199,10 +1215,10 @@
       <c r="B20" s="0" t="n">
         <v>2002</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="4" t="n">
         <v>680983</v>
       </c>
     </row>
@@ -1213,10 +1229,10 @@
       <c r="B21" s="0" t="n">
         <v>2002</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="4" t="n">
         <v>349902</v>
       </c>
     </row>
@@ -1227,10 +1243,10 @@
       <c r="B22" s="0" t="n">
         <v>1991</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="4" t="n">
         <v>527492</v>
       </c>
     </row>
@@ -1241,10 +1257,10 @@
       <c r="B23" s="0" t="n">
         <v>1995</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="4" t="n">
         <v>625620</v>
       </c>
     </row>
@@ -1255,10 +1271,10 @@
       <c r="B24" s="0" t="n">
         <v>1968</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="4" t="n">
         <v>145769</v>
       </c>
     </row>
@@ -1269,10 +1285,10 @@
       <c r="B25" s="0" t="n">
         <v>1942</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="4" t="n">
         <v>278743</v>
       </c>
     </row>
@@ -1283,10 +1299,10 @@
       <c r="B26" s="0" t="n">
         <v>1995</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="4" t="n">
         <v>481594</v>
       </c>
     </row>
@@ -1297,10 +1313,10 @@
       <c r="B27" s="0" t="n">
         <v>1981</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="4" t="n">
         <v>439557</v>
       </c>
     </row>
@@ -1311,10 +1327,10 @@
       <c r="B28" s="0" t="n">
         <v>1954</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="4" t="n">
         <v>213122</v>
       </c>
     </row>
@@ -1325,10 +1341,10 @@
       <c r="B29" s="0" t="n">
         <v>1946</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="4" t="n">
         <v>180212</v>
       </c>
     </row>
@@ -1339,10 +1355,10 @@
       <c r="B30" s="0" t="n">
         <v>1960</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="4" t="n">
         <v>272065</v>
       </c>
     </row>
@@ -1353,10 +1369,10 @@
       <c r="B31" s="0" t="n">
         <v>1994</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="4" t="n">
         <v>454516</v>
       </c>
     </row>
@@ -1367,10 +1383,10 @@
       <c r="B32" s="0" t="n">
         <v>1950</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="4" t="n">
         <v>95571</v>
       </c>
     </row>
@@ -1381,10 +1397,10 @@
       <c r="B33" s="0" t="n">
         <v>1998</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="4" t="n">
         <v>495932</v>
       </c>
     </row>
@@ -1395,10 +1411,10 @@
       <c r="B34" s="0" t="n">
         <v>1979</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="4" t="n">
         <v>309699</v>
       </c>
     </row>
@@ -1409,10 +1425,10 @@
       <c r="B35" s="0" t="n">
         <v>1991</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="4" t="n">
         <v>479572</v>
       </c>
     </row>
@@ -1423,10 +1439,10 @@
       <c r="B36" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="4" t="n">
         <v>557394</v>
       </c>
     </row>
@@ -1437,10 +1453,10 @@
       <c r="B37" s="0" t="n">
         <v>1998</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="4" t="n">
         <v>546922</v>
       </c>
     </row>
@@ -1451,10 +1467,10 @@
       <c r="B38" s="0" t="n">
         <v>1931</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D38" s="4" t="n">
         <v>62840</v>
       </c>
     </row>
@@ -1465,10 +1481,10 @@
       <c r="B39" s="0" t="n">
         <v>1964</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="4" t="n">
         <v>249013</v>
       </c>
     </row>
@@ -1479,10 +1495,10 @@
       <c r="B40" s="0" t="n">
         <v>1979</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="0" t="n">
+      <c r="D40" s="4" t="n">
         <v>360007</v>
       </c>
     </row>
@@ -1493,10 +1509,10 @@
       <c r="B41" s="0" t="n">
         <v>1936</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="D41" s="4" t="n">
         <v>80077</v>
       </c>
     </row>
@@ -1507,10 +1523,10 @@
       <c r="B42" s="0" t="n">
         <v>2001</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="D42" s="4" t="n">
         <v>244430</v>
       </c>
     </row>
@@ -1521,10 +1537,10 @@
       <c r="B43" s="0" t="n">
         <v>2013</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43" s="4" t="n">
         <v>33721</v>
       </c>
     </row>
@@ -1535,10 +1551,10 @@
       <c r="B44" s="0" t="n">
         <v>1959</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="D44" s="4" t="n">
         <v>155574</v>
       </c>
     </row>
@@ -1549,10 +1565,10 @@
       <c r="B45" s="0" t="n">
         <v>1985</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D45" s="0" t="n">
+      <c r="D45" s="4" t="n">
         <v>433401</v>
       </c>
     </row>
@@ -1563,10 +1579,10 @@
       <c r="B46" s="0" t="n">
         <v>1941</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="0" t="n">
+      <c r="D46" s="4" t="n">
         <v>216576</v>
       </c>
     </row>
@@ -1577,10 +1593,10 @@
       <c r="B47" s="0" t="n">
         <v>2002</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D47" s="0" t="n">
+      <c r="D47" s="4" t="n">
         <v>297265</v>
       </c>
     </row>
@@ -1591,10 +1607,10 @@
       <c r="B48" s="0" t="n">
         <v>1931</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="0" t="n">
+      <c r="D48" s="4" t="n">
         <v>68920</v>
       </c>
     </row>
@@ -1605,10 +1621,10 @@
       <c r="B49" s="0" t="n">
         <v>1997</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="0" t="n">
+      <c r="D49" s="4" t="n">
         <v>237603</v>
       </c>
     </row>
@@ -1619,10 +1635,10 @@
       <c r="B50" s="0" t="n">
         <v>1980</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="0" t="n">
+      <c r="D50" s="4" t="n">
         <v>380225</v>
       </c>
     </row>
@@ -1633,10 +1649,10 @@
       <c r="B51" s="0" t="n">
         <v>2006</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D51" s="0" t="n">
+      <c r="D51" s="4" t="n">
         <v>540726</v>
       </c>
     </row>
@@ -1647,10 +1663,10 @@
       <c r="B52" s="0" t="n">
         <v>1957</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D52" s="0" t="n">
+      <c r="D52" s="4" t="n">
         <v>78867</v>
       </c>
     </row>
@@ -1661,10 +1677,10 @@
       <c r="B53" s="0" t="n">
         <v>1958</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D53" s="0" t="n">
+      <c r="D53" s="4" t="n">
         <v>162865</v>
       </c>
     </row>
@@ -1675,10 +1691,10 @@
       <c r="B54" s="0" t="n">
         <v>1999</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D54" s="0" t="n">
+      <c r="D54" s="4" t="n">
         <v>555796</v>
       </c>
     </row>
@@ -1689,10 +1705,10 @@
       <c r="B55" s="0" t="n">
         <v>2012</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="0" t="n">
+      <c r="D55" s="4" t="n">
         <v>450505</v>
       </c>
     </row>
@@ -1703,10 +1719,10 @@
       <c r="B56" s="0" t="n">
         <v>1944</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D56" s="0" t="n">
+      <c r="D56" s="4" t="n">
         <v>66255</v>
       </c>
     </row>
@@ -1717,10 +1733,10 @@
       <c r="B57" s="0" t="n">
         <v>1976</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D57" s="0" t="n">
+      <c r="D57" s="4" t="n">
         <v>321465</v>
       </c>
     </row>
@@ -1731,10 +1747,10 @@
       <c r="B58" s="0" t="n">
         <v>2012</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D58" s="0" t="n">
+      <c r="D58" s="4" t="n">
         <v>672751</v>
       </c>
     </row>
@@ -1745,10 +1761,10 @@
       <c r="B59" s="0" t="n">
         <v>1986</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D59" s="0" t="n">
+      <c r="D59" s="4" t="n">
         <v>325439</v>
       </c>
     </row>
@@ -1759,10 +1775,10 @@
       <c r="B60" s="0" t="n">
         <v>1999</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D60" s="0" t="n">
+      <c r="D60" s="4" t="n">
         <v>447680</v>
       </c>
     </row>
@@ -1773,10 +1789,10 @@
       <c r="B61" s="0" t="n">
         <v>2011</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D61" s="0" t="n">
+      <c r="D61" s="4" t="n">
         <v>223271</v>
       </c>
     </row>
@@ -1787,10 +1803,10 @@
       <c r="B62" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D62" s="0" t="n">
+      <c r="D62" s="4" t="n">
         <v>598332</v>
       </c>
     </row>
@@ -1801,10 +1817,10 @@
       <c r="B63" s="0" t="n">
         <v>2008</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D63" s="0" t="n">
+      <c r="D63" s="4" t="n">
         <v>430863</v>
       </c>
     </row>
@@ -1815,10 +1831,10 @@
       <c r="B64" s="0" t="n">
         <v>2006</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D64" s="0" t="n">
+      <c r="D64" s="4" t="n">
         <v>168022</v>
       </c>
     </row>
@@ -1829,10 +1845,10 @@
       <c r="B65" s="0" t="n">
         <v>2010</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D65" s="0" t="n">
+      <c r="D65" s="4" t="n">
         <v>320991</v>
       </c>
     </row>
@@ -1843,10 +1859,10 @@
       <c r="B66" s="0" t="n">
         <v>1940</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D66" s="0" t="n">
+      <c r="D66" s="4" t="n">
         <v>78329</v>
       </c>
     </row>
@@ -1857,10 +1873,10 @@
       <c r="B67" s="0" t="n">
         <v>1971</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D67" s="0" t="n">
+      <c r="D67" s="4" t="n">
         <v>356779</v>
       </c>
     </row>
@@ -1871,10 +1887,10 @@
       <c r="B68" s="0" t="n">
         <v>2006</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D68" s="0" t="n">
+      <c r="D68" s="4" t="n">
         <v>497983</v>
       </c>
     </row>
@@ -1885,10 +1901,10 @@
       <c r="B69" s="0" t="n">
         <v>2001</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D69" s="0" t="n">
+      <c r="D69" s="4" t="n">
         <v>351134</v>
       </c>
     </row>
@@ -1899,10 +1915,10 @@
       <c r="B70" s="0" t="n">
         <v>1962</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D70" s="0" t="n">
+      <c r="D70" s="4" t="n">
         <v>130531</v>
       </c>
     </row>
@@ -1913,10 +1929,10 @@
       <c r="B71" s="0" t="n">
         <v>1962</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D71" s="0" t="n">
+      <c r="D71" s="4" t="n">
         <v>143215</v>
       </c>
     </row>
@@ -1927,10 +1943,10 @@
       <c r="B72" s="0" t="n">
         <v>1992</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D72" s="0" t="n">
+      <c r="D72" s="4" t="n">
         <v>416840</v>
       </c>
     </row>
@@ -1941,10 +1957,10 @@
       <c r="B73" s="0" t="n">
         <v>1981</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D73" s="0" t="n">
+      <c r="D73" s="4" t="n">
         <v>118641</v>
       </c>
     </row>
@@ -1955,10 +1971,10 @@
       <c r="B74" s="0" t="n">
         <v>1988</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D74" s="0" t="n">
+      <c r="D74" s="4" t="n">
         <v>93024</v>
       </c>
     </row>
@@ -1969,10 +1985,10 @@
       <c r="B75" s="0" t="n">
         <v>1994</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D75" s="0" t="n">
+      <c r="D75" s="4" t="n">
         <v>361740</v>
       </c>
     </row>
@@ -1983,10 +1999,10 @@
       <c r="B76" s="0" t="n">
         <v>1948</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D76" s="0" t="n">
+      <c r="D76" s="4" t="n">
         <v>55469</v>
       </c>
     </row>
@@ -1997,10 +2013,10 @@
       <c r="B77" s="0" t="n">
         <v>1949</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D77" s="0" t="n">
+      <c r="D77" s="4" t="n">
         <v>81076</v>
       </c>
     </row>
@@ -2011,10 +2027,10 @@
       <c r="B78" s="0" t="n">
         <v>1984</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D78" s="0" t="n">
+      <c r="D78" s="4" t="n">
         <v>146293</v>
       </c>
     </row>
@@ -2025,10 +2041,10 @@
       <c r="B79" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D79" s="0" t="n">
+      <c r="D79" s="4" t="n">
         <v>378814</v>
       </c>
     </row>
@@ -2039,10 +2055,10 @@
       <c r="B80" s="0" t="n">
         <v>1983</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D80" s="0" t="n">
+      <c r="D80" s="4" t="n">
         <v>410111</v>
       </c>
     </row>
@@ -2053,10 +2069,10 @@
       <c r="B81" s="0" t="n">
         <v>2004</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D81" s="0" t="n">
+      <c r="D81" s="4" t="n">
         <v>437665</v>
       </c>
     </row>
@@ -2067,10 +2083,10 @@
       <c r="B82" s="0" t="n">
         <v>1987</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D82" s="0" t="n">
+      <c r="D82" s="4" t="n">
         <v>305714</v>
       </c>
     </row>
@@ -2081,10 +2097,10 @@
       <c r="B83" s="0" t="n">
         <v>1995</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D83" s="0" t="n">
+      <c r="D83" s="4" t="n">
         <v>480170</v>
       </c>
     </row>
@@ -2095,10 +2111,10 @@
       <c r="B84" s="0" t="n">
         <v>1997</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D84" s="0" t="n">
+      <c r="D84" s="4" t="n">
         <v>296956</v>
       </c>
     </row>
@@ -2109,10 +2125,10 @@
       <c r="B85" s="0" t="n">
         <v>2003</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D85" s="0" t="n">
+      <c r="D85" s="4" t="n">
         <v>217584</v>
       </c>
     </row>
@@ -2123,10 +2139,10 @@
       <c r="B86" s="0" t="n">
         <v>1952</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D86" s="0" t="n">
+      <c r="D86" s="4" t="n">
         <v>99981</v>
       </c>
     </row>
@@ -2137,10 +2153,10 @@
       <c r="B87" s="0" t="n">
         <v>1927</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D87" s="0" t="n">
+      <c r="D87" s="4" t="n">
         <v>74994</v>
       </c>
     </row>
@@ -2151,10 +2167,10 @@
       <c r="B88" s="0" t="n">
         <v>1974</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D88" s="0" t="n">
+      <c r="D88" s="4" t="n">
         <v>147914</v>
       </c>
     </row>
@@ -2165,10 +2181,10 @@
       <c r="B89" s="0" t="n">
         <v>1950</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D89" s="0" t="n">
+      <c r="D89" s="4" t="n">
         <v>69011</v>
       </c>
     </row>
@@ -2179,10 +2195,10 @@
       <c r="B90" s="0" t="n">
         <v>1959</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D90" s="0" t="n">
+      <c r="D90" s="4" t="n">
         <v>120126</v>
       </c>
     </row>
@@ -2193,10 +2209,10 @@
       <c r="B91" s="0" t="n">
         <v>1948</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D91" s="0" t="n">
+      <c r="D91" s="4" t="n">
         <v>57490</v>
       </c>
     </row>
@@ -2207,10 +2223,10 @@
       <c r="B92" s="0" t="n">
         <v>1950</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D92" s="0" t="n">
+      <c r="D92" s="4" t="n">
         <v>57417</v>
       </c>
     </row>
@@ -2221,10 +2237,10 @@
       <c r="B93" s="0" t="n">
         <v>1975</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D93" s="0" t="n">
+      <c r="D93" s="4" t="n">
         <v>265075</v>
       </c>
     </row>
@@ -2235,10 +2251,10 @@
       <c r="B94" s="0" t="n">
         <v>1997</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D94" s="0" t="n">
+      <c r="D94" s="4" t="n">
         <v>135618</v>
       </c>
     </row>
@@ -2249,10 +2265,10 @@
       <c r="B95" s="0" t="n">
         <v>1984</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C95" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D95" s="0" t="n">
+      <c r="D95" s="4" t="n">
         <v>183169</v>
       </c>
     </row>
@@ -2263,10 +2279,10 @@
       <c r="B96" s="0" t="n">
         <v>1968</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D96" s="0" t="n">
+      <c r="D96" s="4" t="n">
         <v>275055</v>
       </c>
     </row>
@@ -2277,10 +2293,10 @@
       <c r="B97" s="0" t="n">
         <v>1957</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D97" s="0" t="n">
+      <c r="D97" s="4" t="n">
         <v>36241</v>
       </c>
     </row>
@@ -2291,10 +2307,10 @@
       <c r="B98" s="0" t="n">
         <v>1960</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C98" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D98" s="0" t="n">
+      <c r="D98" s="4" t="n">
         <v>70921</v>
       </c>
     </row>
@@ -2305,10 +2321,10 @@
       <c r="B99" s="0" t="n">
         <v>1973</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D99" s="0" t="n">
+      <c r="D99" s="4" t="n">
         <v>117819</v>
       </c>
     </row>
@@ -2319,10 +2335,10 @@
       <c r="B100" s="0" t="n">
         <v>1992</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C100" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D100" s="0" t="n">
+      <c r="D100" s="4" t="n">
         <v>190549</v>
       </c>
     </row>
@@ -2333,10 +2349,10 @@
       <c r="B101" s="0" t="n">
         <v>1988</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D101" s="0" t="n">
+      <c r="D101" s="4" t="n">
         <v>75713</v>
       </c>
     </row>
@@ -2347,10 +2363,10 @@
       <c r="B102" s="0" t="n">
         <v>1989</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D102" s="0" t="n">
+      <c r="D102" s="4" t="n">
         <v>336055</v>
       </c>
     </row>
@@ -2361,10 +2377,10 @@
       <c r="B103" s="0" t="n">
         <v>1980</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D103" s="0" t="n">
+      <c r="D103" s="4" t="n">
         <v>160636</v>
       </c>
     </row>
@@ -2375,10 +2391,10 @@
       <c r="B104" s="0" t="n">
         <v>1957</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C104" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D104" s="0" t="n">
+      <c r="D104" s="4" t="n">
         <v>102421</v>
       </c>
     </row>
@@ -2389,10 +2405,10 @@
       <c r="B105" s="0" t="n">
         <v>1988</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="C105" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D105" s="0" t="n">
+      <c r="D105" s="4" t="n">
         <v>395178</v>
       </c>
     </row>
@@ -2403,10 +2419,10 @@
       <c r="B106" s="0" t="n">
         <v>1961</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D106" s="0" t="n">
+      <c r="D106" s="4" t="n">
         <v>49855</v>
       </c>
     </row>
@@ -2417,10 +2433,10 @@
       <c r="B107" s="0" t="n">
         <v>2005</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C107" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D107" s="0" t="n">
+      <c r="D107" s="4" t="n">
         <v>604923</v>
       </c>
     </row>
@@ -2431,10 +2447,10 @@
       <c r="B108" s="0" t="n">
         <v>2011</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C108" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D108" s="0" t="n">
+      <c r="D108" s="4" t="n">
         <v>93088</v>
       </c>
     </row>
@@ -2445,10 +2461,10 @@
       <c r="B109" s="0" t="n">
         <v>2009</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C109" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D109" s="0" t="n">
+      <c r="D109" s="4" t="n">
         <v>505702</v>
       </c>
     </row>
@@ -2459,10 +2475,10 @@
       <c r="B110" s="0" t="n">
         <v>1965</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="C110" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D110" s="0" t="n">
+      <c r="D110" s="4" t="n">
         <v>94509</v>
       </c>
     </row>
@@ -2473,10 +2489,10 @@
       <c r="B111" s="0" t="n">
         <v>1939</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C111" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D111" s="0" t="n">
+      <c r="D111" s="4" t="n">
         <v>54505</v>
       </c>
     </row>
@@ -2487,10 +2503,10 @@
       <c r="B112" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C112" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D112" s="0" t="n">
+      <c r="D112" s="4" t="n">
         <v>392241</v>
       </c>
     </row>
@@ -2501,10 +2517,10 @@
       <c r="B113" s="0" t="n">
         <v>1995</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D113" s="0" t="n">
+      <c r="D113" s="4" t="n">
         <v>369869</v>
       </c>
     </row>
@@ -2515,10 +2531,10 @@
       <c r="B114" s="0" t="n">
         <v>1954</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C114" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D114" s="0" t="n">
+      <c r="D114" s="4" t="n">
         <v>68966</v>
       </c>
     </row>
@@ -2529,10 +2545,10 @@
       <c r="B115" s="0" t="n">
         <v>1963</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D115" s="0" t="n">
+      <c r="D115" s="4" t="n">
         <v>110551</v>
       </c>
     </row>
@@ -2543,10 +2559,10 @@
       <c r="B116" s="0" t="n">
         <v>2004</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D116" s="0" t="n">
+      <c r="D116" s="4" t="n">
         <v>168689</v>
       </c>
     </row>
@@ -2557,10 +2573,10 @@
       <c r="B117" s="0" t="n">
         <v>2006</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D117" s="0" t="n">
+      <c r="D117" s="4" t="n">
         <v>313115</v>
       </c>
     </row>
@@ -2571,10 +2587,10 @@
       <c r="B118" s="0" t="n">
         <v>2009</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C118" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D118" s="0" t="n">
+      <c r="D118" s="4" t="n">
         <v>377485</v>
       </c>
     </row>
@@ -2585,10 +2601,10 @@
       <c r="B119" s="0" t="n">
         <v>1926</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C119" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D119" s="0" t="n">
+      <c r="D119" s="4" t="n">
         <v>34819</v>
       </c>
     </row>
@@ -2599,10 +2615,10 @@
       <c r="B120" s="0" t="n">
         <v>1957</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C120" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D120" s="0" t="n">
+      <c r="D120" s="4" t="n">
         <v>74369</v>
       </c>
     </row>
@@ -2613,10 +2629,10 @@
       <c r="B121" s="0" t="n">
         <v>1995</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C121" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D121" s="0" t="n">
+      <c r="D121" s="4" t="n">
         <v>297114</v>
       </c>
     </row>
@@ -2627,10 +2643,10 @@
       <c r="B122" s="0" t="n">
         <v>1980</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D122" s="0" t="n">
+      <c r="D122" s="4" t="n">
         <v>111071</v>
       </c>
     </row>
@@ -2641,10 +2657,10 @@
       <c r="B123" s="0" t="n">
         <v>1941</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C123" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D123" s="0" t="n">
+      <c r="D123" s="4" t="n">
         <v>81135</v>
       </c>
     </row>
@@ -2655,10 +2671,10 @@
       <c r="B124" s="0" t="n">
         <v>1921</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C124" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D124" s="0" t="n">
+      <c r="D124" s="4" t="n">
         <v>35316</v>
       </c>
     </row>
@@ -2669,10 +2685,10 @@
       <c r="B125" s="0" t="n">
         <v>1982</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="C125" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D125" s="0" t="n">
+      <c r="D125" s="4" t="n">
         <v>326683</v>
       </c>
     </row>
@@ -2683,10 +2699,10 @@
       <c r="B126" s="0" t="n">
         <v>1957</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D126" s="0" t="n">
+      <c r="D126" s="4" t="n">
         <v>41744</v>
       </c>
     </row>
@@ -2697,10 +2713,10 @@
       <c r="B127" s="0" t="n">
         <v>1940</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="C127" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D127" s="0" t="n">
+      <c r="D127" s="4" t="n">
         <v>61069</v>
       </c>
     </row>
@@ -2711,10 +2727,10 @@
       <c r="B128" s="0" t="n">
         <v>1983</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C128" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D128" s="0" t="n">
+      <c r="D128" s="4" t="n">
         <v>344351</v>
       </c>
     </row>
@@ -2725,10 +2741,10 @@
       <c r="B129" s="0" t="n">
         <v>1952</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D129" s="0" t="n">
+      <c r="D129" s="4" t="n">
         <v>27215</v>
       </c>
     </row>
@@ -2739,10 +2755,10 @@
       <c r="B130" s="0" t="n">
         <v>1985</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C130" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D130" s="0" t="n">
+      <c r="D130" s="4" t="n">
         <v>55197</v>
       </c>
     </row>
@@ -2753,10 +2769,10 @@
       <c r="B131" s="0" t="n">
         <v>1996</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C131" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D131" s="0" t="n">
+      <c r="D131" s="4" t="n">
         <v>285542</v>
       </c>
     </row>
@@ -2767,10 +2783,10 @@
       <c r="B132" s="0" t="n">
         <v>2008</v>
       </c>
-      <c r="C132" s="2" t="s">
+      <c r="C132" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D132" s="0" t="n">
+      <c r="D132" s="4" t="n">
         <v>367352</v>
       </c>
     </row>
@@ -2781,10 +2797,10 @@
       <c r="B133" s="0" t="n">
         <v>1958</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D133" s="0" t="n">
+      <c r="D133" s="4" t="n">
         <v>52508</v>
       </c>
     </row>
@@ -2795,10 +2811,10 @@
       <c r="B134" s="0" t="n">
         <v>1998</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C134" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D134" s="0" t="n">
+      <c r="D134" s="4" t="n">
         <v>348568</v>
       </c>
     </row>
@@ -2809,10 +2825,10 @@
       <c r="B135" s="0" t="n">
         <v>1925</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C135" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D135" s="0" t="n">
+      <c r="D135" s="4" t="n">
         <v>41458</v>
       </c>
     </row>
@@ -2823,10 +2839,10 @@
       <c r="B136" s="0" t="n">
         <v>1978</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D136" s="0" t="n">
+      <c r="D136" s="4" t="n">
         <v>161747</v>
       </c>
     </row>
@@ -2837,10 +2853,10 @@
       <c r="B137" s="0" t="n">
         <v>1967</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="C137" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D137" s="0" t="n">
+      <c r="D137" s="4" t="n">
         <v>84470</v>
       </c>
     </row>
@@ -2851,10 +2867,10 @@
       <c r="B138" s="0" t="n">
         <v>1934</v>
       </c>
-      <c r="C138" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D138" s="0" t="n">
+      <c r="C138" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D138" s="4" t="n">
         <v>43205</v>
       </c>
     </row>
@@ -2865,10 +2881,10 @@
       <c r="B139" s="0" t="n">
         <v>1955</v>
       </c>
-      <c r="C139" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D139" s="0" t="n">
+      <c r="C139" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D139" s="4" t="n">
         <v>26777</v>
       </c>
     </row>
@@ -2879,10 +2895,10 @@
       <c r="B140" s="0" t="n">
         <v>2007</v>
       </c>
-      <c r="C140" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D140" s="0" t="n">
+      <c r="C140" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D140" s="4" t="n">
         <v>397628</v>
       </c>
     </row>
@@ -2893,10 +2909,10 @@
       <c r="B141" s="0" t="n">
         <v>1999</v>
       </c>
-      <c r="C141" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D141" s="0" t="n">
+      <c r="C141" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D141" s="4" t="n">
         <v>475862</v>
       </c>
     </row>
@@ -2907,10 +2923,10 @@
       <c r="B142" s="0" t="n">
         <v>1975</v>
       </c>
-      <c r="C142" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D142" s="0" t="n">
+      <c r="C142" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D142" s="4" t="n">
         <v>267827</v>
       </c>
     </row>
@@ -2921,10 +2937,10 @@
       <c r="B143" s="0" t="n">
         <v>1997</v>
       </c>
-      <c r="C143" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D143" s="0" t="n">
+      <c r="C143" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D143" s="4" t="n">
         <v>366430</v>
       </c>
     </row>
@@ -2935,10 +2951,10 @@
       <c r="B144" s="0" t="n">
         <v>1951</v>
       </c>
-      <c r="C144" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D144" s="0" t="n">
+      <c r="C144" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D144" s="4" t="n">
         <v>64124</v>
       </c>
     </row>
@@ -2949,10 +2965,10 @@
       <c r="B145" s="0" t="n">
         <v>1995</v>
       </c>
-      <c r="C145" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D145" s="0" t="n">
+      <c r="C145" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D145" s="4" t="n">
         <v>216669</v>
       </c>
     </row>
@@ -2963,10 +2979,10 @@
       <c r="B146" s="0" t="n">
         <v>1961</v>
       </c>
-      <c r="C146" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D146" s="0" t="n">
+      <c r="C146" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D146" s="4" t="n">
         <v>25742</v>
       </c>
     </row>
@@ -2977,10 +2993,10 @@
       <c r="B147" s="0" t="n">
         <v>1940</v>
       </c>
-      <c r="C147" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D147" s="0" t="n">
+      <c r="C147" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D147" s="4" t="n">
         <v>42227</v>
       </c>
     </row>
@@ -2991,10 +3007,10 @@
       <c r="B148" s="0" t="n">
         <v>1939</v>
       </c>
-      <c r="C148" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D148" s="0" t="n">
+      <c r="C148" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D148" s="4" t="n">
         <v>192425</v>
       </c>
     </row>
@@ -3005,10 +3021,10 @@
       <c r="B149" s="0" t="n">
         <v>1986</v>
       </c>
-      <c r="C149" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D149" s="0" t="n">
+      <c r="C149" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D149" s="4" t="n">
         <v>202044</v>
       </c>
     </row>
@@ -3019,10 +3035,10 @@
       <c r="B150" s="0" t="n">
         <v>2005</v>
       </c>
-      <c r="C150" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D150" s="0" t="n">
+      <c r="C150" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D150" s="4" t="n">
         <v>459794</v>
       </c>
     </row>
@@ -3033,10 +3049,10 @@
       <c r="B151" s="0" t="n">
         <v>1969</v>
       </c>
-      <c r="C151" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D151" s="0" t="n">
+      <c r="C151" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D151" s="4" t="n">
         <v>102995</v>
       </c>
     </row>
@@ -3047,10 +3063,10 @@
       <c r="B152" s="0" t="n">
         <v>2003</v>
       </c>
-      <c r="C152" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D152" s="0" t="n">
+      <c r="C152" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D152" s="4" t="n">
         <v>470244</v>
       </c>
     </row>
@@ -3061,10 +3077,10 @@
       <c r="B153" s="0" t="n">
         <v>1982</v>
       </c>
-      <c r="C153" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D153" s="0" t="n">
+      <c r="C153" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D153" s="4" t="n">
         <v>175041</v>
       </c>
     </row>
@@ -3075,10 +3091,10 @@
       <c r="B154" s="0" t="n">
         <v>1996</v>
       </c>
-      <c r="C154" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D154" s="0" t="n">
+      <c r="C154" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D154" s="4" t="n">
         <v>312510</v>
       </c>
     </row>
@@ -3089,10 +3105,10 @@
       <c r="B155" s="0" t="n">
         <v>1939</v>
       </c>
-      <c r="C155" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D155" s="0" t="n">
+      <c r="C155" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D155" s="4" t="n">
         <v>148410</v>
       </c>
     </row>
@@ -3103,10 +3119,10 @@
       <c r="B156" s="0" t="n">
         <v>1952</v>
       </c>
-      <c r="C156" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D156" s="0" t="n">
+      <c r="C156" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D156" s="4" t="n">
         <v>56791</v>
       </c>
     </row>
@@ -3117,10 +3133,10 @@
       <c r="B157" s="0" t="n">
         <v>1977</v>
       </c>
-      <c r="C157" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D157" s="0" t="n">
+      <c r="C157" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D157" s="4" t="n">
         <v>127072</v>
       </c>
     </row>
@@ -3131,10 +3147,10 @@
       <c r="B158" s="0" t="n">
         <v>2004</v>
       </c>
-      <c r="C158" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D158" s="0" t="n">
+      <c r="C158" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D158" s="4" t="n">
         <v>180270</v>
       </c>
     </row>
@@ -3145,10 +3161,10 @@
       <c r="B159" s="0" t="n">
         <v>2012</v>
       </c>
-      <c r="C159" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D159" s="0" t="n">
+      <c r="C159" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D159" s="4" t="n">
         <v>39033</v>
       </c>
     </row>
@@ -3159,10 +3175,10 @@
       <c r="B160" s="0" t="n">
         <v>2011</v>
       </c>
-      <c r="C160" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D160" s="0" t="n">
+      <c r="C160" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D160" s="4" t="n">
         <v>190877</v>
       </c>
     </row>
@@ -3173,10 +3189,10 @@
       <c r="B161" s="0" t="n">
         <v>2009</v>
       </c>
-      <c r="C161" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D161" s="0" t="n">
+      <c r="C161" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D161" s="4" t="n">
         <v>73505</v>
       </c>
     </row>
@@ -3187,10 +3203,10 @@
       <c r="B162" s="0" t="n">
         <v>2003</v>
       </c>
-      <c r="C162" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D162" s="0" t="n">
+      <c r="C162" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D162" s="4" t="n">
         <v>406678</v>
       </c>
     </row>
@@ -3201,10 +3217,10 @@
       <c r="B163" s="0" t="n">
         <v>1988</v>
       </c>
-      <c r="C163" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D163" s="0" t="n">
+      <c r="C163" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D163" s="4" t="n">
         <v>88095</v>
       </c>
     </row>
@@ -3215,10 +3231,10 @@
       <c r="B164" s="0" t="n">
         <v>2005</v>
       </c>
-      <c r="C164" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D164" s="0" t="n">
+      <c r="C164" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D164" s="4" t="n">
         <v>507750</v>
       </c>
     </row>
@@ -3229,10 +3245,10 @@
       <c r="B165" s="0" t="n">
         <v>1946</v>
       </c>
-      <c r="C165" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D165" s="0" t="n">
+      <c r="C165" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D165" s="4" t="n">
         <v>52582</v>
       </c>
     </row>
@@ -3243,10 +3259,10 @@
       <c r="B166" s="0" t="n">
         <v>1954</v>
       </c>
-      <c r="C166" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D166" s="0" t="n">
+      <c r="C166" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D166" s="4" t="n">
         <v>65745</v>
       </c>
     </row>
@@ -3257,10 +3273,10 @@
       <c r="B167" s="0" t="n">
         <v>2012</v>
       </c>
-      <c r="C167" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D167" s="0" t="n">
+      <c r="C167" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D167" s="4" t="n">
         <v>568037</v>
       </c>
     </row>
@@ -3271,10 +3287,10 @@
       <c r="B168" s="0" t="n">
         <v>2010</v>
       </c>
-      <c r="C168" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D168" s="0" t="n">
+      <c r="C168" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D168" s="4" t="n">
         <v>249971</v>
       </c>
     </row>
@@ -3285,10 +3301,10 @@
       <c r="B169" s="0" t="n">
         <v>1979</v>
       </c>
-      <c r="C169" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D169" s="0" t="n">
+      <c r="C169" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D169" s="4" t="n">
         <v>183277</v>
       </c>
     </row>
@@ -3299,10 +3315,10 @@
       <c r="B170" s="0" t="n">
         <v>2007</v>
       </c>
-      <c r="C170" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D170" s="0" t="n">
+      <c r="C170" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D170" s="4" t="n">
         <v>263344</v>
       </c>
     </row>
@@ -3313,10 +3329,10 @@
       <c r="B171" s="0" t="n">
         <v>1946</v>
       </c>
-      <c r="C171" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D171" s="0" t="n">
+      <c r="C171" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D171" s="4" t="n">
         <v>27843</v>
       </c>
     </row>
@@ -3327,10 +3343,10 @@
       <c r="B172" s="0" t="n">
         <v>1976</v>
       </c>
-      <c r="C172" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D172" s="0" t="n">
+      <c r="C172" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D172" s="4" t="n">
         <v>69929</v>
       </c>
     </row>
@@ -3341,10 +3357,10 @@
       <c r="B173" s="0" t="n">
         <v>1984</v>
       </c>
-      <c r="C173" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D173" s="0" t="n">
+      <c r="C173" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D173" s="4" t="n">
         <v>378300</v>
       </c>
     </row>
@@ -3355,10 +3371,10 @@
       <c r="B174" s="0" t="n">
         <v>2004</v>
       </c>
-      <c r="C174" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D174" s="0" t="n">
+      <c r="C174" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D174" s="4" t="n">
         <v>303571</v>
       </c>
     </row>
@@ -3369,10 +3385,10 @@
       <c r="B175" s="0" t="n">
         <v>2007</v>
       </c>
-      <c r="C175" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D175" s="0" t="n">
+      <c r="C175" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D175" s="4" t="n">
         <v>252241</v>
       </c>
     </row>
@@ -3383,10 +3399,10 @@
       <c r="B176" s="0" t="n">
         <v>1959</v>
       </c>
-      <c r="C176" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D176" s="0" t="n">
+      <c r="C176" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D176" s="4" t="n">
         <v>106455</v>
       </c>
     </row>
@@ -3397,10 +3413,10 @@
       <c r="B177" s="0" t="n">
         <v>1955</v>
       </c>
-      <c r="C177" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D177" s="0" t="n">
+      <c r="C177" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D177" s="4" t="n">
         <v>44437</v>
       </c>
     </row>
@@ -3411,10 +3427,10 @@
       <c r="B178" s="0" t="n">
         <v>1946</v>
       </c>
-      <c r="C178" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D178" s="0" t="n">
+      <c r="C178" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D178" s="4" t="n">
         <v>47119</v>
       </c>
     </row>
@@ -3425,10 +3441,10 @@
       <c r="B179" s="0" t="n">
         <v>2010</v>
       </c>
-      <c r="C179" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D179" s="0" t="n">
+      <c r="C179" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D179" s="4" t="n">
         <v>288159</v>
       </c>
     </row>
@@ -3439,10 +3455,10 @@
       <c r="B180" s="0" t="n">
         <v>1986</v>
       </c>
-      <c r="C180" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D180" s="0" t="n">
+      <c r="C180" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D180" s="4" t="n">
         <v>182230</v>
       </c>
     </row>
@@ -3453,10 +3469,10 @@
       <c r="B181" s="0" t="n">
         <v>1959</v>
       </c>
-      <c r="C181" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D181" s="0" t="n">
+      <c r="C181" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D181" s="4" t="n">
         <v>46028</v>
       </c>
     </row>
@@ -3467,10 +3483,10 @@
       <c r="B182" s="0" t="n">
         <v>1995</v>
       </c>
-      <c r="C182" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D182" s="0" t="n">
+      <c r="C182" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D182" s="4" t="n">
         <v>316945</v>
       </c>
     </row>
@@ -3481,10 +3497,10 @@
       <c r="B183" s="0" t="n">
         <v>1993</v>
       </c>
-      <c r="C183" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D183" s="0" t="n">
+      <c r="C183" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D183" s="4" t="n">
         <v>282250</v>
       </c>
     </row>
@@ -3498,7 +3514,7 @@
       <c r="C184" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D184" s="0" t="n">
+      <c r="D184" s="4" t="n">
         <v>398128</v>
       </c>
     </row>
@@ -3512,7 +3528,7 @@
       <c r="C185" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D185" s="0" t="n">
+      <c r="D185" s="4" t="n">
         <v>126624</v>
       </c>
     </row>
@@ -3526,7 +3542,7 @@
       <c r="C186" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D186" s="0" t="n">
+      <c r="D186" s="4" t="n">
         <v>120868</v>
       </c>
     </row>
@@ -3540,7 +3556,7 @@
       <c r="C187" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D187" s="0" t="n">
+      <c r="D187" s="4" t="n">
         <v>121059</v>
       </c>
     </row>
@@ -3554,7 +3570,7 @@
       <c r="C188" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D188" s="0" t="n">
+      <c r="D188" s="4" t="n">
         <v>67759</v>
       </c>
     </row>
@@ -3568,7 +3584,7 @@
       <c r="C189" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D189" s="0" t="n">
+      <c r="D189" s="4" t="n">
         <v>110584</v>
       </c>
     </row>
@@ -3582,7 +3598,7 @@
       <c r="C190" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D190" s="0" t="n">
+      <c r="D190" s="4" t="n">
         <v>322172</v>
       </c>
     </row>
@@ -3596,7 +3612,7 @@
       <c r="C191" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D191" s="0" t="n">
+      <c r="D191" s="4" t="n">
         <v>344294</v>
       </c>
     </row>
@@ -3610,7 +3626,7 @@
       <c r="C192" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D192" s="0" t="n">
+      <c r="D192" s="4" t="n">
         <v>36479</v>
       </c>
     </row>
@@ -3624,7 +3640,7 @@
       <c r="C193" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D193" s="0" t="n">
+      <c r="D193" s="4" t="n">
         <v>44571</v>
       </c>
     </row>
@@ -3638,7 +3654,7 @@
       <c r="C194" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D194" s="0" t="n">
+      <c r="D194" s="4" t="n">
         <v>149389</v>
       </c>
     </row>
@@ -3652,7 +3668,7 @@
       <c r="C195" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D195" s="0" t="n">
+      <c r="D195" s="4" t="n">
         <v>28676</v>
       </c>
     </row>
@@ -3666,7 +3682,7 @@
       <c r="C196" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D196" s="0" t="n">
+      <c r="D196" s="4" t="n">
         <v>373745</v>
       </c>
     </row>
@@ -3680,7 +3696,7 @@
       <c r="C197" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D197" s="0" t="n">
+      <c r="D197" s="4" t="n">
         <v>207589</v>
       </c>
     </row>
@@ -3694,7 +3710,7 @@
       <c r="C198" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D198" s="0" t="n">
+      <c r="D198" s="4" t="n">
         <v>38192</v>
       </c>
     </row>
@@ -3708,7 +3724,7 @@
       <c r="C199" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D199" s="0" t="n">
+      <c r="D199" s="4" t="n">
         <v>43710</v>
       </c>
     </row>
@@ -3722,7 +3738,7 @@
       <c r="C200" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D200" s="0" t="n">
+      <c r="D200" s="4" t="n">
         <v>39917</v>
       </c>
     </row>
@@ -3736,7 +3752,7 @@
       <c r="C201" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D201" s="0" t="n">
+      <c r="D201" s="4" t="n">
         <v>32409</v>
       </c>
     </row>
@@ -3750,7 +3766,7 @@
       <c r="C202" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D202" s="0" t="n">
+      <c r="D202" s="4" t="n">
         <v>32242</v>
       </c>
     </row>
@@ -3764,7 +3780,7 @@
       <c r="C203" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D203" s="0" t="n">
+      <c r="D203" s="4" t="n">
         <v>54451</v>
       </c>
     </row>
@@ -3778,7 +3794,7 @@
       <c r="C204" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D204" s="0" t="n">
+      <c r="D204" s="4" t="n">
         <v>53501</v>
       </c>
     </row>
@@ -3792,7 +3808,7 @@
       <c r="C205" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D205" s="0" t="n">
+      <c r="D205" s="4" t="n">
         <v>220323</v>
       </c>
     </row>
@@ -3806,7 +3822,7 @@
       <c r="C206" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D206" s="0" t="n">
+      <c r="D206" s="4" t="n">
         <v>213984</v>
       </c>
     </row>
@@ -3820,7 +3836,7 @@
       <c r="C207" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D207" s="0" t="n">
+      <c r="D207" s="4" t="n">
         <v>425904</v>
       </c>
     </row>
@@ -3834,7 +3850,7 @@
       <c r="C208" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D208" s="0" t="n">
+      <c r="D208" s="4" t="n">
         <v>65291</v>
       </c>
     </row>
@@ -3848,7 +3864,7 @@
       <c r="C209" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D209" s="0" t="n">
+      <c r="D209" s="4" t="n">
         <v>33518</v>
       </c>
     </row>
@@ -3862,7 +3878,7 @@
       <c r="C210" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D210" s="0" t="n">
+      <c r="D210" s="4" t="n">
         <v>66041</v>
       </c>
     </row>
@@ -3876,7 +3892,7 @@
       <c r="C211" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D211" s="0" t="n">
+      <c r="D211" s="4" t="n">
         <v>51331</v>
       </c>
     </row>
@@ -3890,7 +3906,7 @@
       <c r="C212" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D212" s="0" t="n">
+      <c r="D212" s="4" t="n">
         <v>69583</v>
       </c>
     </row>
@@ -3904,7 +3920,7 @@
       <c r="C213" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D213" s="0" t="n">
+      <c r="D213" s="4" t="n">
         <v>27430</v>
       </c>
     </row>
@@ -3918,7 +3934,7 @@
       <c r="C214" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D214" s="0" t="n">
+      <c r="D214" s="4" t="n">
         <v>63858</v>
       </c>
     </row>
@@ -3932,7 +3948,7 @@
       <c r="C215" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D215" s="0" t="n">
+      <c r="D215" s="4" t="n">
         <v>407875</v>
       </c>
     </row>
@@ -3946,7 +3962,7 @@
       <c r="C216" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D216" s="0" t="n">
+      <c r="D216" s="4" t="n">
         <v>63443</v>
       </c>
     </row>
@@ -3960,7 +3976,7 @@
       <c r="C217" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D217" s="0" t="n">
+      <c r="D217" s="4" t="n">
         <v>246325</v>
       </c>
     </row>
@@ -3974,7 +3990,7 @@
       <c r="C218" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D218" s="0" t="n">
+      <c r="D218" s="4" t="n">
         <v>519625</v>
       </c>
     </row>
@@ -3988,7 +4004,7 @@
       <c r="C219" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D219" s="0" t="n">
+      <c r="D219" s="4" t="n">
         <v>33873</v>
       </c>
     </row>
@@ -4002,7 +4018,7 @@
       <c r="C220" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D220" s="0" t="n">
+      <c r="D220" s="4" t="n">
         <v>38373</v>
       </c>
     </row>
@@ -4016,7 +4032,7 @@
       <c r="C221" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D221" s="0" t="n">
+      <c r="D221" s="4" t="n">
         <v>303847</v>
       </c>
     </row>
@@ -4030,7 +4046,7 @@
       <c r="C222" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D222" s="0" t="n">
+      <c r="D222" s="4" t="n">
         <v>30643</v>
       </c>
     </row>
@@ -4044,7 +4060,7 @@
       <c r="C223" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D223" s="0" t="n">
+      <c r="D223" s="4" t="n">
         <v>43524</v>
       </c>
     </row>
@@ -4058,7 +4074,7 @@
       <c r="C224" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D224" s="0" t="n">
+      <c r="D224" s="4" t="n">
         <v>344256</v>
       </c>
     </row>
@@ -4072,7 +4088,7 @@
       <c r="C225" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D225" s="0" t="n">
+      <c r="D225" s="4" t="n">
         <v>60767</v>
       </c>
     </row>
@@ -4086,7 +4102,7 @@
       <c r="C226" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D226" s="0" t="n">
+      <c r="D226" s="4" t="n">
         <v>362442</v>
       </c>
     </row>
@@ -4100,7 +4116,7 @@
       <c r="C227" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D227" s="0" t="n">
+      <c r="D227" s="4" t="n">
         <v>316890</v>
       </c>
     </row>
@@ -4114,7 +4130,7 @@
       <c r="C228" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D228" s="0" t="n">
+      <c r="D228" s="4" t="n">
         <v>86593</v>
       </c>
     </row>
@@ -4128,7 +4144,7 @@
       <c r="C229" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D229" s="0" t="n">
+      <c r="D229" s="4" t="n">
         <v>82374</v>
       </c>
     </row>
@@ -4142,7 +4158,7 @@
       <c r="C230" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D230" s="0" t="n">
+      <c r="D230" s="4" t="n">
         <v>69702</v>
       </c>
     </row>
@@ -4156,7 +4172,7 @@
       <c r="C231" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D231" s="0" t="n">
+      <c r="D231" s="4" t="n">
         <v>352517</v>
       </c>
     </row>
@@ -4170,7 +4186,7 @@
       <c r="C232" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D232" s="0" t="n">
+      <c r="D232" s="4" t="n">
         <v>388592</v>
       </c>
     </row>
@@ -4184,7 +4200,7 @@
       <c r="C233" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D233" s="0" t="n">
+      <c r="D233" s="4" t="n">
         <v>436151</v>
       </c>
     </row>
@@ -4198,7 +4214,7 @@
       <c r="C234" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D234" s="0" t="n">
+      <c r="D234" s="4" t="n">
         <v>276674</v>
       </c>
     </row>
@@ -4212,7 +4228,7 @@
       <c r="C235" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D235" s="0" t="n">
+      <c r="D235" s="4" t="n">
         <v>36751</v>
       </c>
     </row>
@@ -4226,7 +4242,7 @@
       <c r="C236" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D236" s="0" t="n">
+      <c r="D236" s="4" t="n">
         <v>103929</v>
       </c>
     </row>
@@ -4240,7 +4256,7 @@
       <c r="C237" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D237" s="0" t="n">
+      <c r="D237" s="4" t="n">
         <v>63865</v>
       </c>
     </row>
@@ -4254,7 +4270,7 @@
       <c r="C238" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D238" s="0" t="n">
+      <c r="D238" s="4" t="n">
         <v>83178</v>
       </c>
     </row>
@@ -4268,7 +4284,7 @@
       <c r="C239" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D239" s="0" t="n">
+      <c r="D239" s="4" t="n">
         <v>132672</v>
       </c>
     </row>
@@ -4282,7 +4298,7 @@
       <c r="C240" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D240" s="0" t="n">
+      <c r="D240" s="4" t="n">
         <v>53307</v>
       </c>
     </row>
@@ -4293,10 +4309,10 @@
       <c r="B241" s="0" t="n">
         <v>1991</v>
       </c>
-      <c r="C241" s="2" t="s">
+      <c r="C241" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D241" s="0" t="n">
+      <c r="D241" s="4" t="n">
         <v>189229</v>
       </c>
     </row>
@@ -4307,10 +4323,10 @@
       <c r="B242" s="0" t="n">
         <v>1994</v>
       </c>
-      <c r="C242" s="2" t="s">
+      <c r="C242" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D242" s="0" t="n">
+      <c r="D242" s="4" t="n">
         <v>43438</v>
       </c>
     </row>
@@ -4321,10 +4337,10 @@
       <c r="B243" s="0" t="n">
         <v>1938</v>
       </c>
-      <c r="C243" s="2" t="s">
+      <c r="C243" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D243" s="0" t="n">
+      <c r="D243" s="4" t="n">
         <v>35695</v>
       </c>
     </row>
@@ -4335,10 +4351,10 @@
       <c r="B244" s="0" t="n">
         <v>2003</v>
       </c>
-      <c r="C244" s="2" t="s">
+      <c r="C244" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D244" s="0" t="n">
+      <c r="D244" s="4" t="n">
         <v>256159</v>
       </c>
     </row>
@@ -4349,10 +4365,10 @@
       <c r="B245" s="0" t="n">
         <v>1967</v>
       </c>
-      <c r="C245" s="2" t="s">
+      <c r="C245" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D245" s="0" t="n">
+      <c r="D245" s="4" t="n">
         <v>37081</v>
       </c>
     </row>
@@ -4363,10 +4379,10 @@
       <c r="B246" s="0" t="n">
         <v>1944</v>
       </c>
-      <c r="C246" s="2" t="s">
+      <c r="C246" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D246" s="0" t="n">
+      <c r="D246" s="4" t="n">
         <v>45893</v>
       </c>
     </row>
@@ -4377,10 +4393,10 @@
       <c r="B247" s="0" t="n">
         <v>1995</v>
       </c>
-      <c r="C247" s="2" t="s">
+      <c r="C247" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D247" s="0" t="n">
+      <c r="D247" s="4" t="n">
         <v>100974</v>
       </c>
     </row>
@@ -4391,10 +4407,10 @@
       <c r="B248" s="0" t="n">
         <v>1973</v>
       </c>
-      <c r="C248" s="2" t="s">
+      <c r="C248" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D248" s="0" t="n">
+      <c r="D248" s="4" t="n">
         <v>62517</v>
       </c>
     </row>

</xml_diff>